<commit_message>
experimenting with new prompts
</commit_message>
<xml_diff>
--- a/datasets/ucrawler/2023-03-02/2023-03-02_newstags.xlsx
+++ b/datasets/ucrawler/2023-03-02/2023-03-02_newstags.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
   <si>
     <t>Country</t>
   </si>
@@ -46,46 +46,169 @@
     <t>China</t>
   </si>
   <si>
-    <t>Australia</t>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
   </si>
   <si>
     <t>All</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
-    <t>China (1)</t>
-  </si>
-  <si>
-    <t>Australia (1)</t>
-  </si>
-  <si>
-    <t>CATL</t>
-  </si>
-  <si>
-    <t>Pilbara Minerals Ltd</t>
-  </si>
-  <si>
-    <t>Goldman Sachs</t>
-  </si>
-  <si>
-    <t>UBS</t>
-  </si>
-  <si>
-    <t>CATL (1)</t>
-  </si>
-  <si>
-    <t>Pilbara Minerals Ltd (1)</t>
-  </si>
-  <si>
-    <t>Goldman Sachs (1)</t>
-  </si>
-  <si>
-    <t>UBS (1)</t>
+    <t>China (2)</t>
+  </si>
+  <si>
+    <t>Singapore (2)</t>
+  </si>
+  <si>
+    <t>Malaysia (1)</t>
+  </si>
+  <si>
+    <t>Myanmar (1)</t>
+  </si>
+  <si>
+    <t>Japan (1)</t>
+  </si>
+  <si>
+    <t>Vietnam (1)</t>
+  </si>
+  <si>
+    <t>ASEAN</t>
+  </si>
+  <si>
+    <t>Government of Singapore</t>
+  </si>
+  <si>
+    <t>Communist Party of Vietnam</t>
+  </si>
+  <si>
+    <t>National Assembly</t>
+  </si>
+  <si>
+    <t>National water agency PUB</t>
+  </si>
+  <si>
+    <t>National University of Singapore</t>
+  </si>
+  <si>
+    <t>Nanyang Technological University</t>
+  </si>
+  <si>
+    <t>Singapore University of Technology and Design</t>
+  </si>
+  <si>
+    <t>Singapore Institute of Technology</t>
+  </si>
+  <si>
+    <t>Agency for Science</t>
+  </si>
+  <si>
+    <t>ASEAN (1)</t>
+  </si>
+  <si>
+    <t>Government of Singapore (1)</t>
+  </si>
+  <si>
+    <t>Communist Party of Vietnam (1)</t>
+  </si>
+  <si>
+    <t>National Assembly (1)</t>
+  </si>
+  <si>
+    <t>National water agency PUB (1)</t>
+  </si>
+  <si>
+    <t>National University of Singapore (1)</t>
+  </si>
+  <si>
+    <t>Nanyang Technological University (1)</t>
+  </si>
+  <si>
+    <t>Singapore University of Technology and Design (1)</t>
+  </si>
+  <si>
+    <t>Singapore Institute of Technology (1)</t>
+  </si>
+  <si>
+    <t>Agency for Science (1)</t>
+  </si>
+  <si>
+    <t>climate change</t>
+  </si>
+  <si>
+    <t>research programme</t>
+  </si>
+  <si>
+    <t>flood management</t>
+  </si>
+  <si>
+    <t>coastal protection</t>
+  </si>
+  <si>
+    <t>President</t>
+  </si>
+  <si>
+    <t>Vo Van Thuong</t>
+  </si>
+  <si>
+    <t>Silver Generation Office</t>
+  </si>
+  <si>
+    <t>eligibility</t>
+  </si>
+  <si>
+    <t>Annual Value</t>
+  </si>
+  <si>
+    <t>Government social support schemes</t>
+  </si>
+  <si>
+    <t>climate change (1)</t>
+  </si>
+  <si>
+    <t>research programme (1)</t>
+  </si>
+  <si>
+    <t>flood management (1)</t>
+  </si>
+  <si>
+    <t>coastal protection (1)</t>
+  </si>
+  <si>
+    <t>President (1)</t>
+  </si>
+  <si>
+    <t>Vo Van Thuong (1)</t>
+  </si>
+  <si>
+    <t>Silver Generation Office (1)</t>
+  </si>
+  <si>
+    <t>eligibility (1)</t>
+  </si>
+  <si>
+    <t>Annual Value (1)</t>
+  </si>
+  <si>
+    <t>Government social support schemes (1)</t>
   </si>
   <si>
     <t>tags</t>
@@ -450,7 +573,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -496,25 +619,34 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
       </c>
       <c r="J2" s="2">
         <v>44987</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -522,94 +654,313 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="2">
+        <v>44987</v>
+      </c>
+      <c r="K3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="2">
+        <v>44987</v>
+      </c>
+      <c r="K4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="2">
-        <v>44987</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="2">
-        <v>44987</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
       <c r="D5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>58</v>
       </c>
       <c r="J5" s="2">
         <v>44987</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="J6" s="2">
         <v>44987</v>
       </c>
       <c r="K6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="2">
+        <v>44987</v>
+      </c>
+      <c r="K7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="2">
+        <v>44987</v>
+      </c>
+      <c r="K8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="2">
+        <v>44987</v>
+      </c>
+      <c r="K9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="2">
+        <v>44987</v>
+      </c>
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="2">
+        <v>44987</v>
+      </c>
+      <c r="K11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="2">
+        <v>44987</v>
+      </c>
+      <c r="K12" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>